<commit_message>
Archivo Pseudo code modificado para hacer curso de UML
</commit_message>
<xml_diff>
--- a/Guide Web Development.xlsx
+++ b/Guide Web Development.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JEISONDEJESUSANILLOP\Desktop\Jason's data\Web Development\Pseudo_Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JEISONDEJESUSANILLOP\Desktop\Jason's data\Web Development\Projects\Guide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17117C14-BFB1-4247-A720-FD2326A8F461}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE93A63-517F-49D4-ABD4-541E7879D9DC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{7A3AE867-E6A3-422E-92C7-EFDBD7D643A1}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Python</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Step one</t>
+  </si>
+  <si>
+    <t>UML</t>
   </si>
 </sst>
 </file>
@@ -510,7 +513,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,6 +540,9 @@
       <c r="C2" s="8" t="s">
         <v>18</v>
       </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">

</xml_diff>